<commit_message>
+ adjusted wording + updated default weights in bewertungsbogen + made text selectable
</commit_message>
<xml_diff>
--- a/ProStudCreator/Content/Bewertungsbogen_P5_P9.xlsx
+++ b/ProStudCreator/Content/Bewertungsbogen_P5_P9.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de.IRU\Desktop\Bewertung P5 bis P9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de.IRU\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="80" windowWidth="15480" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="2360" yWindow="80" windowWidth="15480" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Beurteilungsbogen (Text)" sheetId="2" r:id="rId1"/>
@@ -713,12 +713,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -739,6 +733,12 @@
       <name val="Wingdings"/>
       <charset val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1513,7 +1513,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1806,15 +1806,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1903,12 +1894,6 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1978,14 +1963,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2147,6 +2132,18 @@
     </xf>
     <xf numFmtId="2" fontId="24" fillId="0" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2156,6 +2153,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2523,358 +2525,358 @@
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" s="175" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="172" t="s">
+    <row r="5" spans="1:5" s="170" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="167" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="173"/>
-      <c r="C5" s="174"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
     </row>
     <row r="6" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="133"/>
-    </row>
-    <row r="7" spans="1:5" s="150" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="149" t="s">
+      <c r="D6" s="130"/>
+    </row>
+    <row r="7" spans="1:5" s="145" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="185" t="s">
+      <c r="B7" s="180" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="186"/>
-      <c r="D7" s="181" t="s">
+      <c r="C7" s="181"/>
+      <c r="D7" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="182" t="s">
+      <c r="E7" s="177" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="183" t="s">
+      <c r="A8" s="178" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="187" t="s">
+      <c r="B8" s="182" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="188"/>
-      <c r="D8" s="189"/>
-      <c r="E8" s="176" t="s">
+      <c r="C8" s="183"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="171" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="150" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="184"/>
-      <c r="B9" s="190"/>
-      <c r="C9" s="191"/>
-      <c r="D9" s="191"/>
-      <c r="E9" s="154">
+    <row r="9" spans="1:5" s="145" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="179"/>
+      <c r="B9" s="185"/>
+      <c r="C9" s="186"/>
+      <c r="D9" s="186"/>
+      <c r="E9" s="149">
         <v>12345</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="150" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="151" t="s">
+    <row r="10" spans="1:5" s="145" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="146" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="209" t="s">
+      <c r="B10" s="204" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="210"/>
-      <c r="D10" s="211"/>
-      <c r="E10" s="177" t="s">
+      <c r="C10" s="205"/>
+      <c r="D10" s="206"/>
+      <c r="E10" s="172" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="150" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="152" t="s">
+    <row r="11" spans="1:5" s="145" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="147" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="179"/>
-      <c r="C11" s="180"/>
-      <c r="D11" s="180"/>
-      <c r="E11" s="178" t="s">
+      <c r="B11" s="174"/>
+      <c r="C11" s="175"/>
+      <c r="D11" s="175"/>
+      <c r="E11" s="173" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="150" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="153" t="s">
+    <row r="12" spans="1:5" s="145" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="148" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="195"/>
-      <c r="C12" s="196"/>
-      <c r="D12" s="196"/>
-      <c r="E12" s="197"/>
+      <c r="B12" s="190"/>
+      <c r="C12" s="191"/>
+      <c r="D12" s="191"/>
+      <c r="E12" s="192"/>
     </row>
     <row r="13" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="120"/>
-      <c r="B13" s="121"/>
+      <c r="A13" s="117"/>
+      <c r="B13" s="118"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" s="150" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="198" t="s">
+    <row r="14" spans="1:5" s="145" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="193" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="199"/>
-      <c r="C14" s="160"/>
-      <c r="D14" s="161"/>
-      <c r="E14" s="162">
+      <c r="B14" s="194"/>
+      <c r="C14" s="155"/>
+      <c r="D14" s="156"/>
+      <c r="E14" s="157">
         <f>Bewertungsbogen!C33</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="129"/>
-      <c r="B15" s="129"/>
-      <c r="C15" s="130"/>
+      <c r="A15" s="126"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="127"/>
       <c r="D15" s="54"/>
-      <c r="E15" s="131"/>
-    </row>
-    <row r="16" spans="1:5" s="150" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="168" t="s">
+      <c r="E15" s="128"/>
+    </row>
+    <row r="16" spans="1:5" s="145" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="163" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="169"/>
-      <c r="C16" s="165"/>
-      <c r="D16" s="166"/>
-      <c r="E16" s="171"/>
-    </row>
-    <row r="17" spans="1:5" s="150" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="200" t="s">
+      <c r="B16" s="164"/>
+      <c r="C16" s="160"/>
+      <c r="D16" s="161"/>
+      <c r="E16" s="166"/>
+    </row>
+    <row r="17" spans="1:5" s="145" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="195" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="201"/>
-      <c r="C17" s="201"/>
-      <c r="D17" s="201"/>
-      <c r="E17" s="202"/>
-    </row>
-    <row r="18" spans="1:5" s="150" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="200" t="s">
+      <c r="B17" s="196"/>
+      <c r="C17" s="196"/>
+      <c r="D17" s="196"/>
+      <c r="E17" s="197"/>
+    </row>
+    <row r="18" spans="1:5" s="145" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="195" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="201"/>
-      <c r="C18" s="201"/>
-      <c r="D18" s="201"/>
-      <c r="E18" s="202"/>
-    </row>
-    <row r="19" spans="1:5" s="150" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="203" t="s">
+      <c r="B18" s="196"/>
+      <c r="C18" s="196"/>
+      <c r="D18" s="196"/>
+      <c r="E18" s="197"/>
+    </row>
+    <row r="19" spans="1:5" s="145" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="198" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="204"/>
-      <c r="C19" s="204"/>
-      <c r="D19" s="204"/>
-      <c r="E19" s="205"/>
+      <c r="B19" s="199"/>
+      <c r="C19" s="199"/>
+      <c r="D19" s="199"/>
+      <c r="E19" s="200"/>
     </row>
     <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="120"/>
-      <c r="B20" s="121"/>
+      <c r="A20" s="117"/>
+      <c r="B20" s="118"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" s="150" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="168" t="s">
+    <row r="21" spans="1:5" s="145" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="163" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="169"/>
-      <c r="C21" s="165"/>
-      <c r="D21" s="166"/>
-      <c r="E21" s="170"/>
-    </row>
-    <row r="22" spans="1:5" s="150" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="206" t="s">
+      <c r="B21" s="164"/>
+      <c r="C21" s="160"/>
+      <c r="D21" s="161"/>
+      <c r="E21" s="165"/>
+    </row>
+    <row r="22" spans="1:5" s="145" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="201" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="207"/>
-      <c r="C22" s="207"/>
-      <c r="D22" s="207"/>
-      <c r="E22" s="208"/>
-    </row>
-    <row r="23" spans="1:5" s="150" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="192" t="s">
+      <c r="B22" s="202"/>
+      <c r="C22" s="202"/>
+      <c r="D22" s="202"/>
+      <c r="E22" s="203"/>
+    </row>
+    <row r="23" spans="1:5" s="145" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="187" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="193"/>
-      <c r="C23" s="193"/>
-      <c r="D23" s="193"/>
-      <c r="E23" s="194"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="188"/>
+      <c r="D23" s="188"/>
+      <c r="E23" s="189"/>
     </row>
     <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:5" s="150" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="163" t="s">
+    <row r="25" spans="1:5" s="145" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="158" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="164"/>
-      <c r="C25" s="165"/>
-      <c r="D25" s="166"/>
-      <c r="E25" s="167"/>
+      <c r="B25" s="159"/>
+      <c r="C25" s="160"/>
+      <c r="D25" s="161"/>
+      <c r="E25" s="162"/>
     </row>
     <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="134"/>
-      <c r="B26" s="122"/>
-      <c r="C26" s="130"/>
+      <c r="A26" s="131"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="127"/>
       <c r="D26" s="54"/>
-      <c r="E26" s="135"/>
+      <c r="E26" s="132"/>
     </row>
     <row r="27" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="134"/>
-      <c r="B27" s="122"/>
-      <c r="C27" s="130"/>
+      <c r="A27" s="131"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="127"/>
       <c r="D27" s="54"/>
-      <c r="E27" s="135"/>
+      <c r="E27" s="132"/>
     </row>
     <row r="28" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="134"/>
-      <c r="B28" s="122"/>
-      <c r="C28" s="130"/>
+      <c r="A28" s="131"/>
+      <c r="B28" s="119"/>
+      <c r="C28" s="127"/>
       <c r="D28" s="54"/>
-      <c r="E28" s="135"/>
+      <c r="E28" s="132"/>
     </row>
     <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="134"/>
-      <c r="B29" s="122"/>
-      <c r="C29" s="130"/>
+      <c r="A29" s="131"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="127"/>
       <c r="D29" s="54"/>
-      <c r="E29" s="135"/>
+      <c r="E29" s="132"/>
     </row>
     <row r="30" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="134"/>
-      <c r="B30" s="122"/>
-      <c r="C30" s="130"/>
+      <c r="A30" s="131"/>
+      <c r="B30" s="119"/>
+      <c r="C30" s="127"/>
       <c r="D30" s="54"/>
-      <c r="E30" s="135"/>
+      <c r="E30" s="132"/>
     </row>
     <row r="31" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="134"/>
-      <c r="B31" s="122"/>
-      <c r="C31" s="130"/>
+      <c r="A31" s="131"/>
+      <c r="B31" s="119"/>
+      <c r="C31" s="127"/>
       <c r="D31" s="54"/>
-      <c r="E31" s="135"/>
+      <c r="E31" s="132"/>
     </row>
     <row r="32" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="134"/>
-      <c r="B32" s="122"/>
-      <c r="C32" s="130"/>
+      <c r="A32" s="131"/>
+      <c r="B32" s="119"/>
+      <c r="C32" s="127"/>
       <c r="D32" s="54"/>
-      <c r="E32" s="135"/>
+      <c r="E32" s="132"/>
     </row>
     <row r="33" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="134"/>
-      <c r="B33" s="122"/>
-      <c r="C33" s="130"/>
+      <c r="A33" s="131"/>
+      <c r="B33" s="119"/>
+      <c r="C33" s="127"/>
       <c r="D33" s="54"/>
-      <c r="E33" s="135"/>
+      <c r="E33" s="132"/>
     </row>
     <row r="34" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="134"/>
-      <c r="B34" s="122"/>
-      <c r="C34" s="130"/>
+      <c r="A34" s="131"/>
+      <c r="B34" s="119"/>
+      <c r="C34" s="127"/>
       <c r="D34" s="54"/>
-      <c r="E34" s="135"/>
+      <c r="E34" s="132"/>
     </row>
     <row r="35" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="134"/>
-      <c r="B35" s="122"/>
-      <c r="C35" s="130"/>
+      <c r="A35" s="131"/>
+      <c r="B35" s="119"/>
+      <c r="C35" s="127"/>
       <c r="D35" s="54"/>
-      <c r="E35" s="135"/>
+      <c r="E35" s="132"/>
     </row>
     <row r="36" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="134"/>
-      <c r="B36" s="122"/>
-      <c r="C36" s="130"/>
+      <c r="A36" s="131"/>
+      <c r="B36" s="119"/>
+      <c r="C36" s="127"/>
       <c r="D36" s="54"/>
-      <c r="E36" s="135"/>
+      <c r="E36" s="132"/>
     </row>
     <row r="37" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="134"/>
-      <c r="B37" s="122"/>
-      <c r="C37" s="130"/>
+      <c r="A37" s="131"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="127"/>
       <c r="D37" s="54"/>
-      <c r="E37" s="135"/>
+      <c r="E37" s="132"/>
     </row>
     <row r="38" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="134"/>
-      <c r="B38" s="122"/>
-      <c r="C38" s="130"/>
+      <c r="A38" s="131"/>
+      <c r="B38" s="119"/>
+      <c r="C38" s="127"/>
       <c r="D38" s="54"/>
-      <c r="E38" s="135"/>
+      <c r="E38" s="132"/>
     </row>
     <row r="39" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="134"/>
-      <c r="B39" s="122"/>
-      <c r="C39" s="130"/>
+      <c r="A39" s="131"/>
+      <c r="B39" s="119"/>
+      <c r="C39" s="127"/>
       <c r="D39" s="54"/>
-      <c r="E39" s="135"/>
+      <c r="E39" s="132"/>
     </row>
     <row r="40" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="134"/>
-      <c r="B40" s="122"/>
-      <c r="C40" s="130"/>
+      <c r="A40" s="131"/>
+      <c r="B40" s="119"/>
+      <c r="C40" s="127"/>
       <c r="D40" s="54"/>
-      <c r="E40" s="135"/>
+      <c r="E40" s="132"/>
     </row>
     <row r="41" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="134"/>
-      <c r="B41" s="122"/>
-      <c r="C41" s="130"/>
+      <c r="A41" s="131"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="127"/>
       <c r="D41" s="54"/>
-      <c r="E41" s="135"/>
+      <c r="E41" s="132"/>
     </row>
     <row r="42" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="134"/>
-      <c r="B42" s="122"/>
-      <c r="C42" s="130"/>
+      <c r="A42" s="131"/>
+      <c r="B42" s="119"/>
+      <c r="C42" s="127"/>
       <c r="D42" s="54"/>
-      <c r="E42" s="135"/>
+      <c r="E42" s="132"/>
     </row>
     <row r="43" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="134"/>
-      <c r="B43" s="122"/>
-      <c r="C43" s="130"/>
+      <c r="A43" s="131"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="127"/>
       <c r="D43" s="54"/>
-      <c r="E43" s="135"/>
+      <c r="E43" s="132"/>
     </row>
     <row r="44" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="134"/>
-      <c r="B44" s="122"/>
-      <c r="C44" s="130"/>
+      <c r="A44" s="131"/>
+      <c r="B44" s="119"/>
+      <c r="C44" s="127"/>
       <c r="D44" s="54"/>
-      <c r="E44" s="135"/>
+      <c r="E44" s="132"/>
     </row>
     <row r="45" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="136"/>
-      <c r="B45" s="137"/>
-      <c r="C45" s="132"/>
-      <c r="D45" s="133"/>
-      <c r="E45" s="138"/>
+      <c r="A45" s="133"/>
+      <c r="B45" s="134"/>
+      <c r="C45" s="129"/>
+      <c r="D45" s="130"/>
+      <c r="E45" s="135"/>
     </row>
     <row r="46" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:5" s="150" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="155" t="s">
+    <row r="47" spans="1:5" s="145" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="156" t="s">
+      <c r="B47" s="151" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="157"/>
-      <c r="D47" s="158" t="s">
+      <c r="C47" s="152"/>
+      <c r="D47" s="153" t="s">
         <v>45</v>
       </c>
-      <c r="E47" s="159"/>
+      <c r="E47" s="154"/>
     </row>
     <row r="48" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="139">
+      <c r="A48" s="136">
         <f ca="1">TODAY()</f>
-        <v>42391</v>
-      </c>
-      <c r="B48" s="143"/>
-      <c r="C48" s="143"/>
+        <v>42501</v>
+      </c>
+      <c r="B48" s="140"/>
+      <c r="C48" s="140"/>
       <c r="D48" s="54"/>
-      <c r="E48" s="140"/>
+      <c r="E48" s="137"/>
     </row>
     <row r="49" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="141"/>
-      <c r="B49" s="144"/>
-      <c r="C49" s="144"/>
-      <c r="D49" s="133"/>
-      <c r="E49" s="142"/>
+      <c r="A49" s="138"/>
+      <c r="B49" s="141"/>
+      <c r="C49" s="141"/>
+      <c r="D49" s="130"/>
+      <c r="E49" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2903,7 +2905,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2919,53 +2921,53 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="212" t="str">
+      <c r="A2" s="207" t="str">
         <f xml:space="preserve"> "Student: " &amp; 'Beurteilungsbogen (Text)'!B7</f>
         <v>Student: xxxxxxxxxx</v>
       </c>
-      <c r="B2" s="213"/>
-      <c r="C2" s="214"/>
-      <c r="D2" s="212" t="str">
+      <c r="B2" s="208"/>
+      <c r="C2" s="209"/>
+      <c r="D2" s="207" t="str">
         <f xml:space="preserve"> "Projekttitel: " &amp; 'Beurteilungsbogen (Text)'!B8</f>
         <v>Projekttitel: yyyyyyyyyyy</v>
       </c>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="214"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="209"/>
     </row>
     <row r="3" spans="1:7" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="215"/>
-      <c r="B3" s="216"/>
-      <c r="C3" s="217"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="216"/>
-      <c r="G3" s="217"/>
+      <c r="A3" s="210"/>
+      <c r="B3" s="211"/>
+      <c r="C3" s="212"/>
+      <c r="D3" s="210"/>
+      <c r="E3" s="211"/>
+      <c r="F3" s="211"/>
+      <c r="G3" s="212"/>
     </row>
     <row r="4" spans="1:7" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="226" t="s">
+      <c r="B4" s="221" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="227"/>
-      <c r="D4" s="227"/>
-      <c r="E4" s="227"/>
-      <c r="F4" s="227"/>
-      <c r="G4" s="227"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
+      <c r="G4" s="222"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="123"/>
-      <c r="B5" s="124"/>
-      <c r="C5" s="125" t="s">
+      <c r="A5" s="120"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="126" t="s">
+      <c r="D5" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="128" t="s">
+      <c r="E5" s="124"/>
+      <c r="F5" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="128" t="s">
+      <c r="G5" s="125" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3178,7 +3180,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="64">
         <v>0</v>
@@ -3194,11 +3196,11 @@
         <f>A18+1</f>
         <v>9</v>
       </c>
-      <c r="B19" s="146" t="s">
+      <c r="B19" s="143" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="147">
-        <v>1</v>
+      <c r="C19" s="225">
+        <v>0.5</v>
       </c>
       <c r="D19" s="70">
         <v>0</v>
@@ -3214,11 +3216,11 @@
         <f>A19+1</f>
         <v>10</v>
       </c>
-      <c r="B20" s="145" t="s">
+      <c r="B20" s="142" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="148">
-        <v>1</v>
+      <c r="C20" s="226">
+        <v>0.5</v>
       </c>
       <c r="D20" s="75">
         <v>0</v>
@@ -3262,7 +3264,7 @@
       <c r="B23" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="112">
+      <c r="C23" s="225">
         <v>1</v>
       </c>
       <c r="D23" s="70">
@@ -3283,7 +3285,7 @@
       <c r="B24" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="113">
+      <c r="C24" s="227">
         <v>1</v>
       </c>
       <c r="D24" s="64">
@@ -3304,7 +3306,7 @@
       <c r="B25" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="114">
+      <c r="C25" s="228">
         <v>1</v>
       </c>
       <c r="D25" s="75">
@@ -3362,10 +3364,10 @@
       <c r="B29" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="220">
+      <c r="C29" s="215">
         <v>0</v>
       </c>
-      <c r="D29" s="221"/>
+      <c r="D29" s="216"/>
       <c r="E29" s="35"/>
       <c r="F29" s="40" t="s">
         <v>27</v>
@@ -3379,10 +3381,10 @@
       <c r="B30" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="222">
+      <c r="C30" s="217">
         <v>0</v>
       </c>
-      <c r="D30" s="223"/>
+      <c r="D30" s="218"/>
       <c r="E30" s="7"/>
       <c r="F30" s="51" t="s">
         <v>24</v>
@@ -3390,32 +3392,32 @@
       <c r="G30" s="51"/>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" ht="38" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="115">
+      <c r="A31" s="112">
         <v>16</v>
       </c>
-      <c r="B31" s="116" t="s">
+      <c r="B31" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="224">
+      <c r="C31" s="219">
         <v>0</v>
       </c>
-      <c r="D31" s="225"/>
-      <c r="E31" s="117"/>
-      <c r="F31" s="118" t="s">
+      <c r="D31" s="220"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="118"/>
+      <c r="G31" s="115"/>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="59"/>
-      <c r="B32" s="119" t="s">
+      <c r="B32" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="228">
+      <c r="C32" s="223">
         <f>0.25*SUM(C29:D31)/30</f>
         <v>0</v>
       </c>
-      <c r="D32" s="229"/>
+      <c r="D32" s="224"/>
       <c r="E32" s="9"/>
       <c r="F32" s="51" t="s">
         <v>32</v>
@@ -3427,11 +3429,11 @@
       <c r="B33" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="218">
+      <c r="C33" s="213">
         <f>ROUND(D27+C32,1)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="219"/>
+      <c r="D33" s="214"/>
       <c r="E33" s="109"/>
       <c r="F33" s="110"/>
       <c r="G33" s="111"/>

</xml_diff>